<commit_message>
Update dossier document avec ajout de tout les doc administratif de BOOKING
</commit_message>
<xml_diff>
--- a/Documents/Méthode MERISE projet pédagogique.xlsx
+++ b/Documents/Méthode MERISE projet pédagogique.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Modèle textuelle des données" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Dictionnaire des données" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="Modèle conceptuel de données" sheetId="2" r:id="rId5"/>
     <sheet state="visible" name="Modèle logique et relationnel d" sheetId="3" r:id="rId6"/>
   </sheets>
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="53">
   <si>
     <t>Nom donnée / Libellé</t>
   </si>
@@ -27,19 +27,19 @@
     <t>adresse_mail</t>
   </si>
   <si>
+    <t>varchar(300)</t>
+  </si>
+  <si>
+    <t>addresse email</t>
+  </si>
+  <si>
+    <t>mail_contenu</t>
+  </si>
+  <si>
     <t>varchar(320)</t>
   </si>
   <si>
-    <t>adresse e-mail de 320 caractère</t>
-  </si>
-  <si>
-    <t>contenu_mail</t>
-  </si>
-  <si>
-    <t>varchar(280)</t>
-  </si>
-  <si>
-    <t>contenu d'un mail</t>
+    <t>contenu du mail</t>
   </si>
   <si>
     <t>num_salle</t>
@@ -51,7 +51,7 @@
     <t>numéro de la salle</t>
   </si>
   <si>
-    <t>date_arriver</t>
+    <t>date_res</t>
   </si>
   <si>
     <t>DATE</t>
@@ -60,12 +60,6 @@
     <t>date d'arriver dans la salle</t>
   </si>
   <si>
-    <t>date_depart</t>
-  </si>
-  <si>
-    <t>date du départ de la salle</t>
-  </si>
-  <si>
     <t>heure_arriver</t>
   </si>
   <si>
@@ -87,16 +81,94 @@
     <t>Temps total réservé pour 1 salle</t>
   </si>
   <si>
+    <t>nom</t>
+  </si>
+  <si>
+    <t>varchar(30)</t>
+  </si>
+  <si>
+    <t>nom de la personne qui réserve</t>
+  </si>
+  <si>
+    <t>prenom</t>
+  </si>
+  <si>
+    <t>prenom de la personne qui réserve</t>
+  </si>
+  <si>
+    <t>poste</t>
+  </si>
+  <si>
+    <t>varchar(50)</t>
+  </si>
+  <si>
+    <t>poste de la personne qui réserve</t>
+  </si>
+  <si>
+    <t>organisation</t>
+  </si>
+  <si>
+    <t>varchar(100)</t>
+  </si>
+  <si>
+    <t>Entreprise/Etablissement de la personne qui réserve</t>
+  </si>
+  <si>
+    <t>date_mail</t>
+  </si>
+  <si>
+    <t>DATETIME</t>
+  </si>
+  <si>
+    <t>Date + heure de réception du mail</t>
+  </si>
+  <si>
+    <t>mdp</t>
+  </si>
+  <si>
+    <t>mot de passe de l'utilisateur ou l'administrateur</t>
+  </si>
+  <si>
+    <t>role_intitule</t>
+  </si>
+  <si>
+    <t>intituler du role de l'utilisateur sur le site</t>
+  </si>
+  <si>
     <t>Modèle conceptuel de données</t>
   </si>
   <si>
+    <t xml:space="preserve">      1:1         </t>
+  </si>
+  <si>
     <t>1:N</t>
   </si>
   <si>
-    <t xml:space="preserve">         0:N</t>
+    <t>1:1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        1:N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         1:1</t>
+  </si>
+  <si>
+    <t>0:1</t>
   </si>
   <si>
     <t>Modèle logique des données</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               1:N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       1:N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       1:1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0:N</t>
   </si>
   <si>
     <t>Modèle rélationnel des données</t>
@@ -106,7 +178,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="8">
+  <fonts count="6">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -114,16 +186,6 @@
     </font>
     <font>
       <b/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="24.0"/>
-    </font>
-    <font>
-      <strike/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
@@ -131,9 +193,14 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="24.0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
     <font/>
     <font>
-      <sz val="24.0"/>
+      <strike/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
@@ -146,13 +213,87 @@
       <patternFill patternType="lightGray"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="11">
     <border/>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
+    <border>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="24">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -163,27 +304,46 @@
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="6" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="7" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="9" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="10" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -201,9 +361,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>704850</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2038350" cy="2438400"/>
     <xdr:grpSp>
@@ -326,23 +486,8 @@
               <a:buNone/>
             </a:pPr>
             <a:r>
-              <a:t/>
-            </a:r>
-            <a:endParaRPr sz="1400"/>
-          </a:p>
-          <a:p>
-            <a:pPr indent="0" lvl="0" marL="0" rtl="0" algn="l">
-              <a:spcBef>
-                <a:spcPts val="0"/>
-              </a:spcBef>
-              <a:spcAft>
-                <a:spcPts val="0"/>
-              </a:spcAft>
-              <a:buNone/>
-            </a:pPr>
-            <a:r>
               <a:rPr lang="en-US" sz="1400"/>
-              <a:t>ma_adresse</a:t>
+              <a:t>ma_id</a:t>
             </a:r>
             <a:endParaRPr sz="1400"/>
           </a:p>
@@ -373,6 +518,37 @@
               <a:buNone/>
             </a:pPr>
             <a:r>
+              <a:rPr lang="en-US" sz="1400"/>
+              <a:t>ma_date</a:t>
+            </a:r>
+            <a:endParaRPr sz="1400"/>
+          </a:p>
+          <a:p>
+            <a:pPr indent="0" lvl="0" marL="0" rtl="0" algn="l">
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buNone/>
+            </a:pPr>
+            <a:r>
+              <a:t/>
+            </a:r>
+            <a:endParaRPr sz="1400"/>
+          </a:p>
+          <a:p>
+            <a:pPr indent="0" lvl="0" marL="0" rtl="0" algn="l">
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buNone/>
+            </a:pPr>
+            <a:r>
               <a:t/>
             </a:r>
             <a:endParaRPr sz="1400"/>
@@ -385,9 +561,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>552450</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1419225" cy="190500"/>
     <xdr:grpSp>
@@ -434,11 +610,11 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>685800</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1619250" cy="2105025"/>
+    <xdr:ext cx="1619250" cy="1066800"/>
     <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="6" name="Shape 6"/>
@@ -447,13 +623,13 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2698150" y="1529275"/>
-          <a:ext cx="1597500" cy="2084400"/>
+          <a:ext cx="1597500" cy="1043100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:srgbClr val="B7B7B7"/>
+          <a:srgbClr val="CCCCCC"/>
         </a:solidFill>
         <a:ln>
           <a:noFill/>
@@ -507,6 +683,22 @@
           </a:pPr>
           <a:r>
             <a:rPr lang="en-US" sz="1400"/>
+            <a:t>sa_id</a:t>
+          </a:r>
+          <a:endParaRPr sz="1400"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="0" lvl="0" marL="0" rtl="0" algn="l">
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400"/>
             <a:t>sa_num</a:t>
           </a:r>
           <a:endParaRPr sz="1400"/>
@@ -517,69 +709,10 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="2105025" cy="904875"/>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="Shape 7"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2444900" y="1626675"/>
-          <a:ext cx="4120200" cy="1763100"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="B7B7B7"/>
-        </a:solidFill>
-        <a:ln cap="flat" cmpd="sng" w="9525">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:round/>
-          <a:headEnd len="sm" w="sm" type="none"/>
-          <a:tailEnd len="sm" w="sm" type="none"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:txBody>
-        <a:bodyPr anchorCtr="0" anchor="ctr" bIns="91425" lIns="91425" spcFirstLastPara="1" rIns="91425" wrap="square" tIns="91425">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr indent="457200" lvl="0" marL="457200" rtl="0" algn="l">
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buNone/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400"/>
-            <a:t>RESERVE</a:t>
-          </a:r>
-          <a:endParaRPr sz="1400"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData fLocksWithSheet="0"/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>771525</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1495425" cy="190500"/>
     <xdr:grpSp>
@@ -597,7 +730,7 @@
       </xdr:grpSpPr>
       <xdr:cxnSp>
         <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="8" name="Shape 8"/>
+          <xdr:cNvPr id="7" name="Shape 7"/>
           <xdr:cNvCxnSpPr/>
         </xdr:nvCxnSpPr>
         <xdr:spPr>
@@ -623,6 +756,832 @@
     </xdr:grpSp>
     <xdr:clientData fLocksWithSheet="0"/>
   </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2047875" cy="1790700"/>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Shape 8"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2931925" y="2201375"/>
+          <a:ext cx="2026200" cy="1638300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="CCCCCC"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr anchorCtr="0" anchor="t" bIns="91425" lIns="91425" spcFirstLastPara="1" rIns="91425" wrap="square" tIns="91425">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr indent="0" lvl="0" marL="0" rtl="0" algn="l">
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400"/>
+            <a:t>RESERVATION</a:t>
+          </a:r>
+          <a:endParaRPr sz="1400"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="0" lvl="0" marL="0" rtl="0" algn="l">
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:t/>
+          </a:r>
+          <a:endParaRPr sz="1400"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="0" lvl="0" marL="0" rtl="0" algn="l">
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400"/>
+            <a:t>res_id</a:t>
+          </a:r>
+          <a:endParaRPr sz="1400"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="0" lvl="0" marL="0" rtl="0" algn="l">
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400"/>
+            <a:t>res_date</a:t>
+          </a:r>
+          <a:endParaRPr sz="1400"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="0" lvl="0" marL="0" rtl="0" algn="l">
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400"/>
+            <a:t>res_heure_arrive</a:t>
+          </a:r>
+          <a:endParaRPr sz="1400"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="0" lvl="0" marL="0" rtl="0" algn="l">
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400"/>
+            <a:t>res_heure_depart</a:t>
+          </a:r>
+          <a:endParaRPr sz="1400"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="0" lvl="0" marL="0" rtl="0" algn="l">
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400"/>
+            <a:t>res_temps_reserver</a:t>
+          </a:r>
+          <a:endParaRPr sz="1400"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="0" lvl="0" marL="0" rtl="0" algn="l">
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:t/>
+          </a:r>
+          <a:endParaRPr sz="1400"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>885825</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1238250" cy="2009775"/>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Shape 9"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2873475" y="2211125"/>
+          <a:ext cx="1685100" cy="2582100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="CCCCCC"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr anchorCtr="0" anchor="t" bIns="91425" lIns="91425" spcFirstLastPara="1" rIns="91425" wrap="square" tIns="91425">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr indent="0" lvl="0" marL="0" rtl="0" algn="l">
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400"/>
+            <a:t>INFORMATION</a:t>
+          </a:r>
+          <a:endParaRPr sz="1400"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="0" lvl="0" marL="0" rtl="0" algn="l">
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:t/>
+          </a:r>
+          <a:endParaRPr sz="1400"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="0" lvl="0" marL="0" rtl="0" algn="l">
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400"/>
+            <a:t>in_id</a:t>
+          </a:r>
+          <a:endParaRPr sz="1400"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="0" lvl="0" marL="0" rtl="0" algn="l">
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400"/>
+            <a:t>in_mail</a:t>
+          </a:r>
+          <a:endParaRPr sz="1400"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="0" lvl="0" marL="0" rtl="0" algn="l">
+            <a:lnSpc>
+              <a:spcPct val="115000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1500"/>
+            <a:t>in_nom</a:t>
+          </a:r>
+          <a:endParaRPr sz="1500"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="0" lvl="0" marL="0" rtl="0" algn="l">
+            <a:lnSpc>
+              <a:spcPct val="115000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1500"/>
+            <a:t>in_prenom</a:t>
+          </a:r>
+          <a:endParaRPr sz="1500"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="0" lvl="0" marL="0" rtl="0" algn="l">
+            <a:lnSpc>
+              <a:spcPct val="115000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1500"/>
+            <a:t>in_poste</a:t>
+          </a:r>
+          <a:endParaRPr sz="1500"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="0" lvl="0" marL="0" rtl="0" algn="l">
+            <a:lnSpc>
+              <a:spcPct val="115000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1500"/>
+            <a:t>in_organisation</a:t>
+          </a:r>
+          <a:endParaRPr sz="1500"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="0" lvl="0" marL="0" rtl="0" algn="l">
+            <a:lnSpc>
+              <a:spcPct val="115000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1500"/>
+            <a:t>in_mdp</a:t>
+          </a:r>
+          <a:endParaRPr sz="1500"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="0" lvl="0" marL="0" rtl="0" algn="l">
+            <a:lnSpc>
+              <a:spcPct val="115000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1500"/>
+            <a:t>role_id</a:t>
+          </a:r>
+          <a:endParaRPr sz="1500"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="0" lvl="0" marL="0" rtl="0" algn="l">
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:t/>
+          </a:r>
+          <a:endParaRPr sz="1400"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="190500" cy="1076325"/>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="2" name="Shape 2" title="Dessin"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="1744900" y="1401800"/>
+          <a:ext cx="0" cy="911700"/>
+          <a:chOff x="1744900" y="1401800"/>
+          <a:chExt cx="0" cy="911700"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp>
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="10" name="Shape 10"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1744900" y="1401800"/>
+            <a:ext cx="0" cy="911700"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln cap="flat" cmpd="sng" w="38100">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+            <a:round/>
+            <a:headEnd len="med" w="med" type="none"/>
+            <a:tailEnd len="med" w="med" type="none"/>
+          </a:ln>
+        </xdr:spPr>
+      </xdr:cxnSp>
+    </xdr:grpSp>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>819150</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1371600" cy="457200"/>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="Shape 11"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2460500" y="1931150"/>
+          <a:ext cx="1349400" cy="441000"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="CFE2F3"/>
+        </a:solidFill>
+        <a:ln cap="flat" cmpd="sng" w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd len="sm" w="sm" type="none"/>
+          <a:tailEnd len="sm" w="sm" type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr anchorCtr="0" anchor="ctr" bIns="91425" lIns="91425" spcFirstLastPara="1" rIns="91425" wrap="square" tIns="91425">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr indent="0" lvl="0" marL="0" rtl="0" algn="l">
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400"/>
+            <a:t>possède</a:t>
+          </a:r>
+          <a:endParaRPr sz="1400"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="990600" cy="571500"/>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="Shape 12"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2372275" y="2303650"/>
+          <a:ext cx="1372500" cy="553800"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="CFE2F3"/>
+        </a:solidFill>
+        <a:ln cap="flat" cmpd="sng" w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd len="sm" w="sm" type="none"/>
+          <a:tailEnd len="sm" w="sm" type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr anchorCtr="0" anchor="ctr" bIns="91425" lIns="91425" spcFirstLastPara="1" rIns="91425" wrap="square" tIns="91425">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr indent="0" lvl="0" marL="0" rtl="0" algn="l">
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400"/>
+            <a:t>réserve</a:t>
+          </a:r>
+          <a:endParaRPr sz="1400"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1076325" cy="457200"/>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="Shape 13"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2372275" y="2303650"/>
+          <a:ext cx="1372500" cy="553800"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="CFE2F3"/>
+        </a:solidFill>
+        <a:ln cap="flat" cmpd="sng" w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd len="sm" w="sm" type="none"/>
+          <a:tailEnd len="sm" w="sm" type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr anchorCtr="0" anchor="ctr" bIns="91425" lIns="91425" spcFirstLastPara="1" rIns="91425" wrap="square" tIns="91425">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr indent="0" lvl="0" marL="0" rtl="0" algn="l">
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400"/>
+            <a:t>demande</a:t>
+          </a:r>
+          <a:endParaRPr sz="1400"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1495425" cy="981075"/>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="Shape 14"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2856550" y="1476850"/>
+          <a:ext cx="1826700" cy="1092300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="B7B7B7"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr anchorCtr="0" anchor="t" bIns="91425" lIns="91425" spcFirstLastPara="1" rIns="91425" wrap="square" tIns="91425">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr indent="0" lvl="0" marL="0" rtl="0" algn="l">
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400"/>
+            <a:t>ROLE</a:t>
+          </a:r>
+          <a:endParaRPr sz="1400"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="0" lvl="0" marL="0" rtl="0" algn="l">
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:t/>
+          </a:r>
+          <a:endParaRPr sz="1400"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="0" lvl="0" marL="0" rtl="0" algn="l">
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400"/>
+            <a:t>role_id</a:t>
+          </a:r>
+          <a:endParaRPr sz="1400"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="0" lvl="0" marL="0" rtl="0" algn="l">
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400"/>
+            <a:t>role_intitule</a:t>
+          </a:r>
+          <a:endParaRPr sz="1400"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1076325" cy="266700"/>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="2" name="Shape 2" title="Dessin"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="1322325" y="2360950"/>
+          <a:ext cx="2000700" cy="88500"/>
+          <a:chOff x="1322325" y="2360950"/>
+          <a:chExt cx="2000700" cy="88500"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp>
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="15" name="Shape 15"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipH="1" rot="10800000">
+            <a:off x="1322325" y="2360950"/>
+            <a:ext cx="2000700" cy="88500"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln cap="flat" cmpd="sng" w="28575">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+            <a:round/>
+            <a:headEnd len="med" w="med" type="none"/>
+            <a:tailEnd len="med" w="med" type="none"/>
+          </a:ln>
+        </xdr:spPr>
+      </xdr:cxnSp>
+    </xdr:grpSp>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="685800" cy="266700"/>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="Shape 16"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2460500" y="1931150"/>
+          <a:ext cx="1620300" cy="441000"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="CFE2F3"/>
+        </a:solidFill>
+        <a:ln cap="flat" cmpd="sng" w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd len="sm" w="sm" type="none"/>
+          <a:tailEnd len="sm" w="sm" type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr anchorCtr="0" anchor="ctr" bIns="91425" lIns="91425" spcFirstLastPara="1" rIns="91425" wrap="square" tIns="91425">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr indent="0" lvl="0" marL="0" rtl="0" algn="l">
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400"/>
+            <a:t>IDENTIFIE</a:t>
+          </a:r>
+          <a:endParaRPr sz="1400"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -631,9 +1590,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>704850</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2038350" cy="2438400"/>
     <xdr:grpSp>
@@ -773,7 +1732,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" sz="1400"/>
-              <a:t>ma_adresse</a:t>
+              <a:t>ma_contenu</a:t>
             </a:r>
             <a:endParaRPr sz="1400"/>
           </a:p>
@@ -789,7 +1748,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" sz="1400"/>
-              <a:t>ma_contenu</a:t>
+              <a:t>ma_date</a:t>
             </a:r>
             <a:endParaRPr sz="1400"/>
           </a:p>
@@ -804,7 +1763,8 @@
               <a:buNone/>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:rPr lang="en-US" sz="1400"/>
+              <a:t>#in_id</a:t>
             </a:r>
             <a:endParaRPr sz="1400"/>
           </a:p>
@@ -816,9 +1776,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>561975</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1419225" cy="190500"/>
     <xdr:grpSp>
@@ -865,11 +1825,11 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>685800</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1619250" cy="2105025"/>
+    <xdr:ext cx="1266825" cy="1276350"/>
     <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="6" name="Shape 6"/>
@@ -878,7 +1838,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2698150" y="1529275"/>
-          <a:ext cx="1597500" cy="2084400"/>
+          <a:ext cx="1246800" cy="1256400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -964,70 +1924,21 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>704850</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>209550</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1905000" cy="190500"/>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="2" name="Shape 2" title="Dessin"/>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="1852725" y="2205625"/>
-          <a:ext cx="1784100" cy="0"/>
-          <a:chOff x="1852725" y="2205625"/>
-          <a:chExt cx="1784100" cy="0"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:cxnSp>
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="8" name="Shape 8"/>
-          <xdr:cNvCxnSpPr/>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="1852725" y="2205625"/>
-            <a:ext cx="1784100" cy="0"/>
-          </a:xfrm>
-          <a:prstGeom prst="straightConnector1">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:ln cap="flat" cmpd="sng" w="38100">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:prstDash val="solid"/>
-            <a:round/>
-            <a:headEnd len="med" w="med" type="none"/>
-            <a:tailEnd len="med" w="med" type="none"/>
-          </a:ln>
-        </xdr:spPr>
-      </xdr:cxnSp>
-    </xdr:grpSp>
-    <xdr:clientData fLocksWithSheet="0"/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="1943100" cy="2181225"/>
+    <xdr:ext cx="1790700" cy="2181225"/>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="Shape 9"/>
+        <xdr:cNvPr id="17" name="Shape 17"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3233875" y="1655900"/>
-          <a:ext cx="1928700" cy="2158500"/>
+          <a:ext cx="1772700" cy="2158500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1087,7 +1998,7 @@
           </a:pPr>
           <a:r>
             <a:rPr b="1" lang="en-US" sz="1400" u="sng"/>
-            <a:t>#sa_id</a:t>
+            <a:t>res_id</a:t>
           </a:r>
           <a:endParaRPr b="1" sz="1400" u="sng"/>
         </a:p>
@@ -1102,40 +2013,8 @@
             <a:buNone/>
           </a:pPr>
           <a:r>
-            <a:rPr b="1" lang="en-US" sz="1400" u="sng"/>
-            <a:t>#ma_id</a:t>
-          </a:r>
-          <a:endParaRPr b="1" sz="1400" u="sng"/>
-        </a:p>
-        <a:p>
-          <a:pPr indent="0" lvl="0" marL="0" rtl="0" algn="l">
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buNone/>
-          </a:pPr>
-          <a:r>
             <a:rPr lang="en-US" sz="1400"/>
-            <a:t>res_date_arrive</a:t>
-          </a:r>
-          <a:endParaRPr sz="1400"/>
-        </a:p>
-        <a:p>
-          <a:pPr indent="0" lvl="0" marL="0" rtl="0" algn="l">
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buNone/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400"/>
-            <a:t>res_date_depart</a:t>
+            <a:t>res_date</a:t>
           </a:r>
           <a:endParaRPr sz="1400"/>
         </a:p>
@@ -1184,6 +2063,38 @@
           <a:r>
             <a:rPr lang="en-US" sz="1400"/>
             <a:t>res_temps_reserve</a:t>
+          </a:r>
+          <a:endParaRPr sz="1400"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="0" lvl="0" marL="0" rtl="0" algn="l">
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400"/>
+            <a:t>#sa_id</a:t>
+          </a:r>
+          <a:endParaRPr sz="1400"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="0" lvl="0" marL="0" rtl="0" algn="l">
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400"/>
+            <a:t>#ma_id</a:t>
           </a:r>
           <a:endParaRPr sz="1400"/>
         </a:p>
@@ -1194,14 +2105,14 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="9525000" cy="1247775"/>
+    <xdr:ext cx="9525000" cy="1257300"/>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="Shape 10"/>
+        <xdr:cNvPr id="18" name="Shape 18"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1235,69 +2146,605 @@
             <a:buNone/>
           </a:pPr>
           <a:r>
-            <a:rPr lang="en-US" sz="1300"/>
+            <a:rPr lang="en-US" sz="1500"/>
             <a:t>MAIL(</a:t>
           </a:r>
           <a:r>
-            <a:rPr b="1" lang="en-US" sz="1300" u="sng"/>
+            <a:rPr b="1" lang="en-US" sz="1500" u="sng"/>
             <a:t>ma_id</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-US" sz="1300"/>
-            <a:t>, ma_adresse, ma_contenu)</a:t>
-          </a:r>
-          <a:endParaRPr sz="1300"/>
-        </a:p>
-        <a:p>
-          <a:pPr indent="0" lvl="0" marL="0" rtl="0" algn="l">
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buNone/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1300"/>
+            <a:rPr lang="en-US" sz="1500"/>
+            <a:t>, ma_contenu, ma_date, #in_id)</a:t>
+          </a:r>
+          <a:endParaRPr sz="1500"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="0" lvl="0" marL="0" rtl="0" algn="l">
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1500"/>
             <a:t>SALLE(</a:t>
           </a:r>
           <a:r>
-            <a:rPr b="1" lang="en-US" sz="1300" u="sng"/>
+            <a:rPr b="1" lang="en-US" sz="1500" u="sng"/>
             <a:t>sa_id</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-US" sz="1300"/>
+            <a:rPr lang="en-US" sz="1500"/>
             <a:t>, sa_name)</a:t>
           </a:r>
-          <a:endParaRPr sz="1300"/>
-        </a:p>
-        <a:p>
-          <a:pPr indent="0" lvl="0" marL="0" rtl="0" algn="l">
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buNone/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1300"/>
+          <a:endParaRPr sz="1500"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="0" lvl="0" marL="0" rtl="0" algn="l">
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1500"/>
             <a:t>RESERVATION(</a:t>
           </a:r>
           <a:r>
-            <a:rPr b="1" lang="en-US" sz="1300" u="sng"/>
+            <a:rPr b="1" lang="en-US" sz="1500" u="sng"/>
+            <a:t>res_id</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1500"/>
+            <a:t>, res_date,  res_heure_arrive, res_heure_depart, res_temps_reserve, </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1500"/>
             <a:t>#sa_id, #ma_id</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-US" sz="1300"/>
-            <a:t>, res_date_arrive, res_date_depart,  res_heure_arrive, res_heure_depart, res_temps_reserve)</a:t>
-          </a:r>
-          <a:endParaRPr sz="1300"/>
+            <a:rPr lang="en-US" sz="1500"/>
+            <a:t>)</a:t>
+          </a:r>
+          <a:endParaRPr sz="1500"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="0" lvl="0" marL="0" rtl="0" algn="l">
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1500"/>
+            <a:t>INFORMATION(</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr b="1" lang="en-US" sz="1500" u="sng"/>
+            <a:t>in_id</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr b="1" lang="en-US" sz="1500"/>
+            <a:t>, </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1500"/>
+            <a:t>in_mail, in_nom, in_prenom, in_poste, in_organisation, #role_id)</a:t>
+          </a:r>
+          <a:endParaRPr sz="1500"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="0" lvl="0" marL="0" rtl="0" algn="l">
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1500"/>
+            <a:t>ROLE(</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr b="1" lang="en-US" sz="1500" u="sng"/>
+            <a:t>role_id</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1500"/>
+            <a:t>, role_intitule)</a:t>
+          </a:r>
+          <a:endParaRPr sz="1500"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1704975" cy="2762250"/>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="19" name="Shape 19"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2873475" y="2211125"/>
+          <a:ext cx="1685100" cy="2504100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="CCCCCC"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr anchorCtr="0" anchor="t" bIns="91425" lIns="91425" spcFirstLastPara="1" rIns="91425" wrap="square" tIns="91425">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr indent="0" lvl="0" marL="0" rtl="0" algn="l">
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400"/>
+            <a:t>INFORMATION</a:t>
+          </a:r>
+          <a:endParaRPr sz="1400"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="0" lvl="0" marL="0" rtl="0" algn="l">
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:t/>
+          </a:r>
+          <a:endParaRPr sz="1400"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="0" lvl="0" marL="0" rtl="0" algn="l">
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="1" lang="en-US" sz="1400" u="sng"/>
+            <a:t>in_id</a:t>
+          </a:r>
+          <a:endParaRPr b="1" sz="1400" u="sng"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="0" lvl="0" marL="0" rtl="0" algn="l">
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400"/>
+            <a:t>in_mail</a:t>
+          </a:r>
+          <a:endParaRPr sz="1400"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="0" lvl="0" marL="0" rtl="0" algn="l">
+            <a:lnSpc>
+              <a:spcPct val="115000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1500"/>
+            <a:t>in_nom</a:t>
+          </a:r>
+          <a:endParaRPr sz="1500"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="0" lvl="0" marL="0" rtl="0" algn="l">
+            <a:lnSpc>
+              <a:spcPct val="115000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1500"/>
+            <a:t>in_prenom</a:t>
+          </a:r>
+          <a:endParaRPr sz="1500"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="0" lvl="0" marL="0" rtl="0" algn="l">
+            <a:lnSpc>
+              <a:spcPct val="115000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1500"/>
+            <a:t>in_poste</a:t>
+          </a:r>
+          <a:endParaRPr sz="1500"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="0" lvl="0" marL="0" rtl="0" algn="l">
+            <a:lnSpc>
+              <a:spcPct val="115000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1500"/>
+            <a:t>in_organisation</a:t>
+          </a:r>
+          <a:endParaRPr sz="1500"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="0" lvl="0" marL="0" rtl="0" algn="l">
+            <a:lnSpc>
+              <a:spcPct val="115000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1500"/>
+            <a:t>in_mdp</a:t>
+          </a:r>
+          <a:endParaRPr sz="1500"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="0" lvl="0" marL="0" rtl="0" algn="l">
+            <a:lnSpc>
+              <a:spcPct val="115000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1500"/>
+            <a:t>#role_id</a:t>
+          </a:r>
+          <a:endParaRPr sz="1500"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="0" lvl="0" marL="0" rtl="0" algn="l">
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:t/>
+          </a:r>
+          <a:endParaRPr sz="1400"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="190500" cy="1190625"/>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="2" name="Shape 2" title="Dessin"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="1205725" y="1393025"/>
+          <a:ext cx="31200" cy="920400"/>
+          <a:chOff x="1205725" y="1393025"/>
+          <a:chExt cx="31200" cy="920400"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp>
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="20" name="Shape 20"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipH="1" rot="10800000">
+            <a:off x="1205725" y="1393025"/>
+            <a:ext cx="31200" cy="920400"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln cap="flat" cmpd="sng" w="28575">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+            <a:round/>
+            <a:headEnd len="med" w="med" type="none"/>
+            <a:tailEnd len="med" w="med" type="none"/>
+          </a:ln>
+        </xdr:spPr>
+      </xdr:cxnSp>
+    </xdr:grpSp>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1476375" cy="1362075"/>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="21" name="Shape 21"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2431075" y="1117525"/>
+          <a:ext cx="1460700" cy="1343100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="CCCCCC"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr anchorCtr="0" anchor="t" bIns="91425" lIns="91425" spcFirstLastPara="1" rIns="91425" wrap="square" tIns="91425">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr indent="0" lvl="0" marL="0" rtl="0" algn="l">
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400"/>
+            <a:t>ROLE</a:t>
+          </a:r>
+          <a:endParaRPr sz="1400"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="0" lvl="0" marL="0" rtl="0" algn="l">
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:t/>
+          </a:r>
+          <a:endParaRPr sz="1400"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="0" lvl="0" marL="0" rtl="0" algn="l">
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="1" lang="en-US" sz="1400" u="sng"/>
+            <a:t>role_id</a:t>
+          </a:r>
+          <a:endParaRPr b="1" sz="1400" u="sng"/>
+        </a:p>
+        <a:p>
+          <a:pPr indent="0" lvl="0" marL="0" rtl="0" algn="l">
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400"/>
+            <a:t>role_intitule</a:t>
+          </a:r>
+          <a:endParaRPr sz="1400"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1476375" cy="190500"/>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="2" name="Shape 2" title="Dessin"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="1205725" y="2313425"/>
+          <a:ext cx="931800" cy="37800"/>
+          <a:chOff x="1205725" y="2313425"/>
+          <a:chExt cx="931800" cy="37800"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp>
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="22" name="Shape 22"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1205725" y="2313425"/>
+            <a:ext cx="931800" cy="37800"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln cap="flat" cmpd="sng" w="28575">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+            <a:round/>
+            <a:headEnd len="med" w="med" type="none"/>
+            <a:tailEnd len="med" w="med" type="none"/>
+          </a:ln>
+        </xdr:spPr>
+      </xdr:cxnSp>
+    </xdr:grpSp>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1876425" cy="190500"/>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="2" name="Shape 2" title="Dessin"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="1205725" y="2303525"/>
+          <a:ext cx="1401900" cy="9900"/>
+          <a:chOff x="1205725" y="2303525"/>
+          <a:chExt cx="1401900" cy="9900"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp>
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="23" name="Shape 23"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipH="1" rot="10800000">
+            <a:off x="1205725" y="2303525"/>
+            <a:ext cx="1401900" cy="9900"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln cap="flat" cmpd="sng" w="28575">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+            <a:round/>
+            <a:headEnd len="med" w="med" type="none"/>
+            <a:tailEnd len="med" w="med" type="none"/>
+          </a:ln>
+        </xdr:spPr>
+      </xdr:cxnSp>
+    </xdr:grpSp>
     <xdr:clientData fLocksWithSheet="0"/>
   </xdr:oneCellAnchor>
 </xdr:wsDr>
@@ -1501,6 +2948,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1508,7 +2956,8 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="28.57"/>
-    <col customWidth="1" min="2" max="3" width="29.14"/>
+    <col customWidth="1" min="2" max="2" width="29.14"/>
+    <col customWidth="1" min="3" max="3" width="45.57"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1523,99 +2972,163 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
+      <c r="A2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>8</v>
+      <c r="A4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>14</v>
+      <c r="A6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="4" t="s">
+      <c r="A7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>16</v>
       </c>
+      <c r="C7" s="3" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>18</v>
+      <c r="A8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>21</v>
+      <c r="A9" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="3" t="s">
+      <c r="A10" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>23</v>
       </c>
+      <c r="C10" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>39</v>
+      </c>
     </row>
   </sheetData>
+  <printOptions gridLines="1" horizontalCentered="1"/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -1630,24 +3143,51 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
+    <row r="2">
+      <c r="E2" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="7"/>
+    </row>
+    <row r="6">
+      <c r="D6" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
     <row r="7">
-      <c r="E7" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F7" s="6"/>
+      <c r="B7" s="8"/>
     </row>
     <row r="8">
-      <c r="F8" s="7"/>
+      <c r="F8" s="9"/>
     </row>
     <row r="9">
-      <c r="F9" s="7"/>
-    </row>
-    <row r="15">
-      <c r="E15" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="H15" s="9" t="s">
-        <v>26</v>
+      <c r="F9" s="9"/>
+    </row>
+    <row r="16">
+      <c r="D16" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="D19" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="D22" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="H22" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="I22" s="6" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1659,6 +3199,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1668,35 +3209,226 @@
     <col customWidth="1" min="12" max="13" width="43.57"/>
   </cols>
   <sheetData>
+    <row r="2">
+      <c r="B2" s="11"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" s="13"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="14"/>
+    </row>
+    <row r="3">
+      <c r="B3" s="15"/>
+      <c r="L3" s="16"/>
+    </row>
+    <row r="4">
+      <c r="B4" s="15"/>
+      <c r="L4" s="16"/>
+    </row>
+    <row r="5">
+      <c r="B5" s="15"/>
+      <c r="L5" s="16"/>
+    </row>
+    <row r="6">
+      <c r="B6" s="15"/>
+      <c r="L6" s="16"/>
+    </row>
     <row r="7">
-      <c r="E7" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" s="10"/>
+      <c r="B7" s="15"/>
+      <c r="D7" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="K7" s="17"/>
+      <c r="L7" s="16"/>
     </row>
     <row r="8">
-      <c r="F8" s="7"/>
+      <c r="B8" s="15"/>
+      <c r="F8" s="9"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="16"/>
     </row>
     <row r="9">
-      <c r="F9" s="7"/>
+      <c r="B9" s="15"/>
+      <c r="F9" s="9"/>
+      <c r="L9" s="16"/>
+    </row>
+    <row r="10">
+      <c r="B10" s="15"/>
+      <c r="L10" s="16"/>
+    </row>
+    <row r="11">
+      <c r="B11" s="15"/>
+      <c r="L11" s="16"/>
+    </row>
+    <row r="12">
+      <c r="B12" s="15"/>
+      <c r="L12" s="16"/>
     </row>
     <row r="13">
-      <c r="L13" s="9"/>
+      <c r="B13" s="15"/>
+      <c r="L13" s="19"/>
+    </row>
+    <row r="14">
+      <c r="B14" s="15"/>
+      <c r="L14" s="16"/>
     </row>
     <row r="15">
-      <c r="E15" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="H15" s="8" t="s">
-        <v>26</v>
-      </c>
+      <c r="B15" s="15"/>
+      <c r="L15" s="16"/>
+    </row>
+    <row r="16">
+      <c r="B16" s="15"/>
+      <c r="D16" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="L16" s="16"/>
+    </row>
+    <row r="17">
+      <c r="B17" s="15"/>
+      <c r="L17" s="16"/>
+    </row>
+    <row r="18">
+      <c r="B18" s="15"/>
+      <c r="L18" s="16"/>
+    </row>
+    <row r="19">
+      <c r="B19" s="15"/>
+      <c r="L19" s="16"/>
+    </row>
+    <row r="20">
+      <c r="B20" s="15"/>
+      <c r="D20" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="L20" s="16"/>
+    </row>
+    <row r="21">
+      <c r="B21" s="15"/>
+      <c r="L21" s="16"/>
+    </row>
+    <row r="22">
+      <c r="B22" s="15"/>
+      <c r="L22" s="16"/>
+    </row>
+    <row r="23">
+      <c r="B23" s="15"/>
+      <c r="L23" s="16"/>
+    </row>
+    <row r="24">
+      <c r="B24" s="15"/>
+      <c r="D24" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="G24" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="L24" s="16"/>
+    </row>
+    <row r="25">
+      <c r="B25" s="15"/>
+      <c r="L25" s="16"/>
     </row>
     <row r="26">
-      <c r="E26" s="10" t="s">
-        <v>28</v>
-      </c>
+      <c r="B26" s="15"/>
+      <c r="L26" s="16"/>
+    </row>
+    <row r="27">
+      <c r="B27" s="15"/>
+      <c r="L27" s="16"/>
+    </row>
+    <row r="28">
+      <c r="B28" s="15"/>
+      <c r="L28" s="16"/>
+    </row>
+    <row r="29">
+      <c r="B29" s="15"/>
+      <c r="L29" s="16"/>
+    </row>
+    <row r="30">
+      <c r="B30" s="15"/>
+      <c r="L30" s="16"/>
+    </row>
+    <row r="31">
+      <c r="B31" s="15"/>
+      <c r="L31" s="16"/>
+    </row>
+    <row r="32">
+      <c r="B32" s="15"/>
+      <c r="L32" s="16"/>
+    </row>
+    <row r="33">
+      <c r="B33" s="15"/>
+      <c r="L33" s="16"/>
+    </row>
+    <row r="34">
+      <c r="B34" s="15"/>
+      <c r="E34" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="L34" s="16"/>
+    </row>
+    <row r="35">
+      <c r="B35" s="15"/>
+      <c r="L35" s="16"/>
+    </row>
+    <row r="36">
+      <c r="B36" s="15"/>
+      <c r="L36" s="16"/>
+    </row>
+    <row r="37">
+      <c r="B37" s="15"/>
+      <c r="L37" s="16"/>
+    </row>
+    <row r="38">
+      <c r="B38" s="15"/>
+      <c r="L38" s="16"/>
+    </row>
+    <row r="39">
+      <c r="B39" s="15"/>
+      <c r="L39" s="16"/>
+    </row>
+    <row r="40">
+      <c r="B40" s="15"/>
+      <c r="L40" s="16"/>
+    </row>
+    <row r="41">
+      <c r="B41" s="15"/>
+      <c r="L41" s="16"/>
+    </row>
+    <row r="42">
+      <c r="B42" s="21"/>
+      <c r="C42" s="22"/>
+      <c r="D42" s="22"/>
+      <c r="E42" s="22"/>
+      <c r="F42" s="22"/>
+      <c r="G42" s="22"/>
+      <c r="H42" s="22"/>
+      <c r="I42" s="22"/>
+      <c r="J42" s="22"/>
+      <c r="K42" s="22"/>
+      <c r="L42" s="23"/>
     </row>
   </sheetData>
+  <printOptions gridLines="1" horizontalCentered="1"/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.25" right="0.25" top="0.75"/>
+  <pageSetup paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>